<commit_message>
Calculate Client Security Hash in RE Framework
</commit_message>
<xml_diff>
--- a/Calculate Client Security Hash/Data/Config.xlsx
+++ b/Calculate Client Security Hash/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\Calculate Client Security Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2B7517-A1DA-42EB-BCC1-9E568D7579A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C7780D-09FC-49E2-9BA6-819FAEC368AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -234,7 +234,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,7 +627,7 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1640,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2803,8 +2802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>